<commit_message>
merging all changes on v5.5.0-rc.10
</commit_message>
<xml_diff>
--- a/Sample.xlsx
+++ b/Sample.xlsx
@@ -14,10 +14,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>EDE: GDP: Current Prices</t>
+    <t>Trade Balance</t>
   </si>
   <si>
-    <t>GDP: Gross Capital Formation (GCF)</t>
+    <t>BoP: Current Account: sa</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
updated files on 5.7.0_rc.1
</commit_message>
<xml_diff>
--- a/Sample.xlsx
+++ b/Sample.xlsx
@@ -14,10 +14,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>Trade Balance</t>
+    <t>EDE: GDP: Current Prices</t>
   </si>
   <si>
-    <t>BoP: Current Account: sa</t>
+    <t>GDP: Gross Capital Formation (GCF)</t>
   </si>
 </sst>
 </file>

</xml_diff>